<commit_message>
Entendiendo un Blend a profundidad
</commit_message>
<xml_diff>
--- a/Tableau/Sección 4; Uniendo y Combinando Datos & Gráficos de Doble Eje/datasets/P1-Airline-Comparison.xlsx
+++ b/Tableau/Sección 4; Uniendo y Combinando Datos & Gráficos de Doble Eje/datasets/P1-Airline-Comparison.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_BB7E8671581B6890B0A49255F8AC264FD37D79C9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{239E244C-41B2-4670-A22A-079E78A6F866}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Airline1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Region</t>
   </si>
@@ -51,16 +52,19 @@
   </si>
   <si>
     <t>FY2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,11 +102,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -144,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +188,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +240,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,20 +433,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:A7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -409,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -420,7 +468,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -431,7 +479,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -442,7 +490,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -453,7 +501,7 @@
         <v>120000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -464,7 +512,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -475,7 +523,7 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -486,7 +534,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -497,7 +545,7 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -508,7 +556,7 @@
         <v>56000000</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -519,7 +567,7 @@
         <v>96000000</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -530,7 +578,7 @@
         <v>120000000</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -539,6 +587,11 @@
       </c>
       <c r="C13" s="1">
         <v>48000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -547,20 +600,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -571,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -582,7 +635,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -593,7 +646,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -604,7 +657,7 @@
         <v>50000000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -615,7 +668,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -626,7 +679,7 @@
         <v>10500000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -637,7 +690,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -648,7 +701,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>

</xml_diff>